<commit_message>
TCHOF Update, Part 1
Added some of the missing leaderboard queries.
</commit_message>
<xml_diff>
--- a/Static/Mass Effect 3 MP TCHOF Challenge Details.xlsx
+++ b/Static/Mass Effect 3 MP TCHOF Challenge Details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MEHOF\Static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DBEE31-8117-4434-83C5-530BA40E3281}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9E5AAF-E4DE-44D8-8661-DD794C524954}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27945" windowHeight="18240" tabRatio="750" firstSheet="20" activeTab="20" xr2:uid="{B39D7FE3-EF3E-44DD-A2C3-49440A173CB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27885" windowHeight="18240" tabRatio="750" firstSheet="20" activeTab="20" xr2:uid="{B39D7FE3-EF3E-44DD-A2C3-49440A173CB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="36" state="hidden" r:id="rId1"/>
@@ -12398,8 +12398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CBA69C-5C1F-4245-943C-878AE74AC996}">
   <dimension ref="A1:AI449"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41429,7 +41429,7 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z449" xr:uid="{D8AF1667-39D8-41D6-A8F9-47FE15D875D7}">
       <formula1>vlRulesCyclonic</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD449" xr:uid="{438D08E9-5585-4AD7-97BD-A05AB803D3E3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD449" xr:uid="{438D08E9-5585-4AD7-97BD-A05AB803D3E3}">
       <formula1>vlRulesGame</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="W2:W449" xr:uid="{593367B1-8985-4BC0-8F20-898689B84FEE}">

</xml_diff>